<commit_message>
Criando o Array para guardar as lojas que estão dando erro
</commit_message>
<xml_diff>
--- a/CadastroCNPJ/Minhas Unidades.xlsx
+++ b/CadastroCNPJ/Minhas Unidades.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7e32da25853bd735/Área de Trabalho/Nova pasta/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7e32da25853bd735/Área de Trabalho/Nova pasta/CadastroCNPJ/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="120" documentId="8_{D703FF8E-40FC-4AD2-AB23-06D77A001340}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{40E26D7A-0664-4141-9625-138EEB958FB4}"/>
+  <xr:revisionPtr revIDLastSave="144" documentId="8_{D703FF8E-40FC-4AD2-AB23-06D77A001340}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F75E209E-4757-43FA-B065-2D331EBBF58D}"/>
   <bookViews>
-    <workbookView xWindow="-24120" yWindow="1575" windowWidth="24240" windowHeight="13020" xr2:uid="{42B77C7D-5F13-4598-8FBB-EE9C3E20BED4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{42B77C7D-5F13-4598-8FBB-EE9C3E20BED4}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
     <t>Nome da Filial</t>
   </si>
@@ -47,16 +47,10 @@
     <t>Fantasia</t>
   </si>
   <si>
-    <t>88.543.679/0001-06</t>
+    <t>93.421.457/0001-50</t>
   </si>
   <si>
-    <t>46.346.081/0001-87</t>
-  </si>
-  <si>
-    <t>TesteCNPJ01</t>
-  </si>
-  <si>
-    <t>TesteCNPJ00</t>
+    <t>Teste</t>
   </si>
 </sst>
 </file>
@@ -421,10 +415,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D0D9622-31EC-4FD3-8FA2-68D1F2266F0C}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -448,26 +442,112 @@
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
-        <v>5</v>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
       </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
       <c r="C8" s="1"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>